<commit_message>
Inicio de front-end angular
</commit_message>
<xml_diff>
--- a/Sistema_gestion_actividades/staticfiles/media/task_finished.xlsx
+++ b/Sistema_gestion_actividades/staticfiles/media/task_finished.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,7 +500,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -509,7 +509,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Crear una app de busqueda</t>
+          <t>Se necesita configurar el ambiente de desarrollo para digitel</t>
         </is>
       </c>
       <c r="D2" t="b">
@@ -531,19 +531,19 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Sistema y tecnologia</t>
+          <t>Departamento de prueba</t>
         </is>
       </c>
       <c r="J2" s="2" t="n">
-        <v>45159</v>
+        <v>45145</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>45160</v>
+        <v>45146</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -552,7 +552,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Crear una app de busqueda</t>
+          <t>Se necesita configurar el ambiente de desarrollo para digitel</t>
         </is>
       </c>
       <c r="D3" t="b">
@@ -574,14 +574,229 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Sistema y tecnologia</t>
+          <t>Departamento de prueba</t>
         </is>
       </c>
       <c r="J3" s="2" t="n">
-        <v>45159</v>
+        <v>45145</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>45160</v>
+        <v>45146</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Tarea para departamento de sistema</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Se necesita configurar el ambiente de desarrollo para digitel</t>
+        </is>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>gabriel1407, user_admin</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Departamento de prueba</t>
+        </is>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>45145</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>45146</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>32</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Tarea para departamento de sistema</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Se necesita configurar el ambiente de desarrollo para digitel</t>
+        </is>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>gabriel1407, user_admin</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Departamento de prueba</t>
+        </is>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>45145</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>45146</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>31</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Tarea para departamento de sistema</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Se necesita configurar el ambiente de desarrollo para digitel</t>
+        </is>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>gabriel1407, user_admin</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Departamento de prueba</t>
+        </is>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>45145</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>45146</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>30</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Tarea para departamento de sistema</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Se necesita configurar el ambiente de desarrollo para digitel</t>
+        </is>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>gabriel1407, user_admin</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Departamento de prueba</t>
+        </is>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>45145</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>45146</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>29</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Tarea para departamento de sistema</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Se necesita subir al repositorio los cambios del Front-end</t>
+        </is>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>gabriel1407, user_admin</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Departamento de prueba</t>
+        </is>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>45139</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>45140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>